<commit_message>
Refactor to fix error on adding new fields
</commit_message>
<xml_diff>
--- a/Processed/Request.xlsx
+++ b/Processed/Request.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\OneDrive\Documents\UiPath\ZohoDesk\Requests\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="14" documentId="8_{5C349E63-42A9-4130-B6F1-AB237975A5FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{7BD38FD7-4810-4497-B6C6-9263FB933C18}"/>
+  <xr:revisionPtr revIDLastSave="18" documentId="8_{5C349E63-42A9-4130-B6F1-AB237975A5FC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{2F8195BC-0003-4950-A93A-1E1839063C0D}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12375" xr2:uid="{F54A0D43-6901-488C-9A14-6CBF4733CBAA}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Contact Name</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Test RPA</t>
+  </si>
+  <si>
+    <t>Phone</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -405,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB7C9A7E-1F11-46BD-9F4D-13B327AB6083}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,6 +447,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4">
+        <v>712345678</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{27E93948-C8E6-4AF6-8886-21F710E24620}"/>

</xml_diff>